<commit_message>
Added data for experiment 3
</commit_message>
<xml_diff>
--- a/Data/A-Ci curves with predicted A-Exp3.xlsx
+++ b/Data/A-Ci curves with predicted A-Exp3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://campusruacza-my.sharepoint.com/personal/g12f2166_campusruacza_onmicrosoft_com/Documents/M.Sc Project/M.Sc Project/Oxailis pes-caprae_Nutrient exp 2017/A-Ci curves/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CO2-effects-on-geophytes\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="341" documentId="114_{93B0BDA3-E8C8-4E03-B4D4-38C963BF7CB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CEEAC198-F753-4730-B219-5210A4F95928}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797E4CF7-BF5F-4747-8723-EB3416F2BD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{CA5E0E91-9171-4DAE-B053-27BFBA02E87E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{CA5E0E91-9171-4DAE-B053-27BFBA02E87E}"/>
   </bookViews>
   <sheets>
     <sheet name="70%" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="24">
   <si>
     <t>Ci</t>
   </si>
@@ -2338,9 +2338,9 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>400</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>300</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>0.87671812361904622</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>200</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>0.90766264937196106</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>100</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>1.5782812095857555</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>50</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>1.8256556680637024</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>400</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>1.8565662064473885</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>500</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>1.7249924366495677</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>600</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>1.6094566380707462</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>700</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>1.523418143249188</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>800</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>1.4694416081439776</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>900</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>1.444919252994801</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>400</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>1.4449034814100068</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>300</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>200</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>100</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>50</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>400</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>500</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>600</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>700</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>800</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>900</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>400</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>300</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>200</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>100</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>50</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>400</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>500</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>600</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>700</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>800</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>900</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>400</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>300</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>200</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>100</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>50</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>400</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>500</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>600</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>700</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>800</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>900</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>400</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>300</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>200</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>100</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>50</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>400</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>500</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>600</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>700</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>800</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>900</v>
       </c>
@@ -3814,9 +3814,9 @@
       <selection activeCell="A2" sqref="A2:E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D1">
         <v>16</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>400</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>-2.9579055779399837</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>300</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>1.8474066314107334</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>200</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>9.8808385968796131</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>100</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>15.258174820296531</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>50</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>17.24990587488896</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>400</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>18.538136362030297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>500</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>19.45067187892765</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>600</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>20.130946627552959</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>700</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>20.657623268577865</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>800</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>21.077445683344258</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>900</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>21.419937449972984</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>400</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>300</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>200</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>0.89631192968602991</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>100</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>0.25124128588477962</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>50</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>1.1990154568848337</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>400</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>1.875333355541871</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>500</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>2.1456172955509878</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>600</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>2.3372454040270365</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>700</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>2.4730570405170185</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>800</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>2.574332717022731</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>900</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>2.6527576269435515</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>400</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>2.715280549634544</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>300</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>2.7662924503571542</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>200</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>100</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>50</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>400</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>500</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>600</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>700</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>800</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>900</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>400</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>300</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>200</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>100</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>50</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>400</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>500</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>600</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>700</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>800</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>900</v>
       </c>
@@ -5074,12 +5074,12 @@
       <selection sqref="A1:E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -5114,7 +5114,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>400</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>300</v>
       </c>
@@ -5227,7 +5227,7 @@
         <v>1.7910925943332374</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>200</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>1.5870783759537896</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>100</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>1.4138832833968751</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>50</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>1.3637550910746163</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>400</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>1.3272730343590669</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>500</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>1.3756646744531202</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>600</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>1.4145955612462267</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>700</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>1.4459177924037991</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>800</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>1.4714285231943505</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>900</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>1.4925102181114767</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>400</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>1.5101783486664817</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>300</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>200</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>100</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>50</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>400</v>
       </c>
@@ -5892,7 +5892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>500</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>600</v>
       </c>
@@ -5926,7 +5926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>700</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>800</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>900</v>
       </c>
@@ -5977,7 +5977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>400</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>300</v>
       </c>
@@ -6011,7 +6011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>200</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>100</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>50</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>400</v>
       </c>
@@ -6079,7 +6079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>500</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>600</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>700</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>800</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>900</v>
       </c>
@@ -6164,7 +6164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>400</v>
       </c>
@@ -6181,7 +6181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>300</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>200</v>
       </c>
@@ -6215,7 +6215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>100</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>50</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>400</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>500</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>600</v>
       </c>
@@ -6300,7 +6300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>700</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>800</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>900</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>400</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>300</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>200</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>100</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>50</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>400</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>500</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>600</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>700</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>800</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>900</v>
       </c>
@@ -6552,9 +6552,9 @@
       <selection sqref="A1:E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -6571,7 +6571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>400</v>
       </c>
@@ -6594,7 +6594,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>300</v>
       </c>
@@ -6617,7 +6617,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>200</v>
       </c>
@@ -6640,7 +6640,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>100</v>
       </c>
@@ -6663,7 +6663,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>50</v>
       </c>
@@ -6686,7 +6686,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>400</v>
       </c>
@@ -6709,7 +6709,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>500</v>
       </c>
@@ -6732,7 +6732,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>600</v>
       </c>
@@ -6755,7 +6755,7 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>700</v>
       </c>
@@ -6778,7 +6778,7 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>800</v>
       </c>
@@ -6801,7 +6801,7 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>900</v>
       </c>
@@ -6824,7 +6824,7 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>400</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>300</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>200</v>
       </c>
@@ -6875,7 +6875,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>100</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>50</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>400</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>500</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>600</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>700</v>
       </c>
@@ -6977,7 +6977,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>800</v>
       </c>
@@ -6994,7 +6994,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>900</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>400</v>
       </c>
@@ -7028,7 +7028,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>300</v>
       </c>
@@ -7045,7 +7045,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>200</v>
       </c>
@@ -7062,7 +7062,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>100</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>50</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>400</v>
       </c>
@@ -7113,7 +7113,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>500</v>
       </c>
@@ -7130,7 +7130,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>600</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>700</v>
       </c>
@@ -7164,7 +7164,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>800</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>900</v>
       </c>
@@ -7198,135 +7198,135 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D35" s="6"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D36" s="6"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D37" s="6"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D38" s="6"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D39" s="6"/>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D40" s="6"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D41" s="6"/>
       <c r="E41" s="4"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D42" s="6"/>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D43" s="6"/>
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D44" s="6"/>
       <c r="E44" s="4"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D45" s="6"/>
       <c r="E45" s="4"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D46" s="6"/>
       <c r="E46" s="4"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D47" s="6"/>
       <c r="E47" s="4"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D48" s="6"/>
       <c r="E48" s="4"/>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D49" s="6"/>
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D50" s="6"/>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D51" s="6"/>
       <c r="E51" s="4"/>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D52" s="6"/>
       <c r="E52" s="4"/>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D53" s="6"/>
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D54" s="6"/>
       <c r="E54" s="4"/>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D55" s="6"/>
       <c r="E55" s="4"/>
     </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D56" s="6"/>
       <c r="E56" s="4"/>
     </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D57" s="6"/>
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D58" s="6"/>
       <c r="E58" s="4"/>
     </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D59" s="6"/>
       <c r="E59" s="4"/>
     </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D60" s="6"/>
       <c r="E60" s="4"/>
     </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D61" s="6"/>
       <c r="E61" s="4"/>
     </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D62" s="6"/>
       <c r="E62" s="4"/>
     </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D63" s="6"/>
       <c r="E63" s="4"/>
     </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D64" s="6"/>
       <c r="E64" s="4"/>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D65" s="6"/>
       <c r="E65" s="4"/>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D66" s="6"/>
       <c r="E66" s="4"/>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D67" s="6"/>
       <c r="E67" s="4"/>
     </row>
@@ -7343,9 +7343,9 @@
       <selection activeCell="M2" sqref="M2:M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>50</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>15.55</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>50</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>15.73</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>50</v>
       </c>
@@ -7485,7 +7485,7 @@
         <v>23.28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>50</v>
       </c>
@@ -7508,7 +7508,7 @@
         <v>1.875333355541871</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>50</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>50</v>
       </c>
@@ -7572,7 +7572,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>50</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>5.41</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>50</v>
       </c>
@@ -7636,7 +7636,7 @@
         <v>2.64</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>50</v>
       </c>
@@ -7659,7 +7659,7 @@
         <v>2.6527576269435515</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>50</v>
       </c>
@@ -7682,7 +7682,7 @@
         <v>2.715280549634544</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>50</v>
       </c>
@@ -7714,7 +7714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>70</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>70</v>
       </c>
@@ -7778,7 +7778,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>70</v>
       </c>
@@ -7810,7 +7810,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>70</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>1.8256556680637024</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>70</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>1.8565662064473885</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>70</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>1.7249924366495677</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>70</v>
       </c>
@@ -7902,7 +7902,7 @@
         <v>1.6094566380707462</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>70</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>1.523418143249188</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>70</v>
       </c>
@@ -7948,7 +7948,7 @@
         <v>1.4694416081439776</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>70</v>
       </c>
@@ -7971,7 +7971,7 @@
         <v>1.444919252994801</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>70</v>
       </c>
@@ -7994,7 +7994,7 @@
         <v>1.4449034814100068</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>100</v>
       </c>
@@ -8017,7 +8017,7 @@
         <v>1.7910925943332374</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>100</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>1.5870783759537896</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>100</v>
       </c>
@@ -8063,7 +8063,7 @@
         <v>1.4138832833968751</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>100</v>
       </c>
@@ -8086,7 +8086,7 @@
         <v>1.3637550910746163</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>100</v>
       </c>
@@ -8109,7 +8109,7 @@
         <v>1.3272730343590669</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>100</v>
       </c>
@@ -8132,7 +8132,7 @@
         <v>1.3756646744531202</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>100</v>
       </c>
@@ -8155,7 +8155,7 @@
         <v>1.4145955612462267</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>100</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>1.4459177924037991</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>100</v>
       </c>
@@ -8201,7 +8201,7 @@
         <v>1.4714285231943505</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>100</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>1.4925102181114767</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>100</v>
       </c>
@@ -8254,21 +8254,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA082BF-324C-409C-9475-FBE41DD98CA6}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1:P7"/>
+      <selection pane="topRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -8309,7 +8309,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8354,7 +8354,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -8399,7 +8399,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4</v>
       </c>
@@ -8444,7 +8444,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
@@ -8478,7 +8478,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>7</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>10</v>
       </c>
@@ -8568,7 +8568,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>11</v>
       </c>
@@ -8604,7 +8604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>12</v>
       </c>
@@ -8629,7 +8629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>13</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>16</v>
       </c>
@@ -8679,7 +8679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>17</v>
       </c>
@@ -8703,8 +8703,20 @@
       <c r="L12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" t="s">
+        <v>16</v>
+      </c>
+      <c r="P12" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>18</v>
       </c>
@@ -8728,8 +8740,20 @@
       <c r="L13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>22.34</v>
+      </c>
+      <c r="O13">
+        <v>26.907191880741671</v>
+      </c>
+      <c r="P13">
+        <v>16.97387040975671</v>
+      </c>
+      <c r="Q13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>19</v>
       </c>
@@ -8753,8 +8777,20 @@
       <c r="L14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>24.58</v>
+      </c>
+      <c r="O14">
+        <v>26.2847228445453</v>
+      </c>
+      <c r="P14">
+        <v>6.4856032708713593</v>
+      </c>
+      <c r="Q14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J15">
         <v>327.74</v>
       </c>
@@ -8764,8 +8800,20 @@
       <c r="L15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>18.07</v>
+      </c>
+      <c r="O15">
+        <v>21.91469362528732</v>
+      </c>
+      <c r="P15">
+        <v>17.54390771336605</v>
+      </c>
+      <c r="Q15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D16" s="6"/>
       <c r="J16">
         <v>220.9</v>
@@ -8776,8 +8824,20 @@
       <c r="L16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>26.97</v>
+      </c>
+      <c r="O16">
+        <v>30.643153324857202</v>
+      </c>
+      <c r="P16">
+        <v>11.986864686923731</v>
+      </c>
+      <c r="Q16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J17">
         <v>224.13</v>
       </c>
@@ -8787,8 +8847,20 @@
       <c r="L17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>25.14</v>
+      </c>
+      <c r="O17">
+        <v>29.095939523975886</v>
+      </c>
+      <c r="P17">
+        <v>13.596191044857234</v>
+      </c>
+      <c r="Q17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J18">
         <v>268.48</v>
       </c>
@@ -8798,8 +8870,20 @@
       <c r="L18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>14.06</v>
+      </c>
+      <c r="O18">
+        <v>16.146089742463584</v>
+      </c>
+      <c r="P18">
+        <v>12.920092578063958</v>
+      </c>
+      <c r="Q18">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J19">
         <v>249.48</v>
       </c>
@@ -8809,8 +8893,20 @@
       <c r="L19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>20.86</v>
+      </c>
+      <c r="O19">
+        <v>22.374683938440562</v>
+      </c>
+      <c r="P19">
+        <v>6.7696327805474716</v>
+      </c>
+      <c r="Q19">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J20">
         <v>157.76</v>
       </c>
@@ -8820,8 +8916,20 @@
       <c r="L20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>17.34</v>
+      </c>
+      <c r="O20">
+        <v>19.004613416840172</v>
+      </c>
+      <c r="P20">
+        <v>8.7589964622229157</v>
+      </c>
+      <c r="Q20">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J21">
         <v>195.36</v>
       </c>
@@ -8831,8 +8939,20 @@
       <c r="L21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>20.99</v>
+      </c>
+      <c r="O21">
+        <v>24.544613416840175</v>
+      </c>
+      <c r="P21">
+        <v>14.482254645743737</v>
+      </c>
+      <c r="Q21">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J22">
         <v>210.42</v>
       </c>
@@ -8842,8 +8962,20 @@
       <c r="L22" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>13.38</v>
+      </c>
+      <c r="O22">
+        <v>14.708529165175698</v>
+      </c>
+      <c r="P22">
+        <v>9.0323726475734745</v>
+      </c>
+      <c r="Q22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J23">
         <v>210.15</v>
       </c>
@@ -8853,8 +8985,20 @@
       <c r="L23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>19.79</v>
+      </c>
+      <c r="O23">
+        <v>22.222107894083997</v>
+      </c>
+      <c r="P23">
+        <v>10.944541830487097</v>
+      </c>
+      <c r="Q23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J24">
         <v>118.76</v>
       </c>
@@ -8864,8 +9008,20 @@
       <c r="L24" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>8.77</v>
+      </c>
+      <c r="O24">
+        <v>9.6722610988238369</v>
+      </c>
+      <c r="P24">
+        <v>9.3283368759922514</v>
+      </c>
+      <c r="Q24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J25">
         <v>219</v>
       </c>
@@ -8875,8 +9031,20 @@
       <c r="L25" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>20.65</v>
+      </c>
+      <c r="O25">
+        <v>22.396725341472301</v>
+      </c>
+      <c r="P25">
+        <v>7.7990211284944806</v>
+      </c>
+      <c r="Q25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J26">
         <v>79.540000000000006</v>
       </c>
@@ -8887,7 +9055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J27">
         <v>220.84</v>
       </c>
@@ -8898,7 +9066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J28">
         <v>15.82</v>
       </c>
@@ -8909,7 +9077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J29">
         <v>4.3</v>
       </c>
@@ -8920,7 +9088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J30">
         <v>8.83</v>
       </c>
@@ -8931,7 +9099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J31">
         <v>5.55</v>
       </c>
@@ -8942,7 +9110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="10:17" x14ac:dyDescent="0.35">
       <c r="J32">
         <v>5.09</v>
       </c>
@@ -8953,7 +9121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J33">
         <v>6.41</v>
       </c>
@@ -8964,7 +9132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J34">
         <v>5.09</v>
       </c>
@@ -8975,7 +9143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J35">
         <v>10.41</v>
       </c>
@@ -8986,7 +9154,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J36">
         <v>4.6399999999999997</v>
       </c>
@@ -8997,7 +9165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J37">
         <v>2.4</v>
       </c>
@@ -9008,7 +9176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J38">
         <v>8.15</v>
       </c>
@@ -9019,7 +9187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J39">
         <v>1.97</v>
       </c>
@@ -9030,7 +9198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J40">
         <v>8.32</v>
       </c>

</xml_diff>

<commit_message>
Updated data for A-Ci curves
</commit_message>
<xml_diff>
--- a/Data/A-Ci curves with predicted A-Exp3.xlsx
+++ b/Data/A-Ci curves with predicted A-Exp3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CO2-effects-on-geophytes\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797E4CF7-BF5F-4747-8723-EB3416F2BD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F734322-8382-4E4C-92AD-E3E316FD81CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{CA5E0E91-9171-4DAE-B053-27BFBA02E87E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="26">
   <si>
     <t>Ci</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>Ls</t>
+  </si>
+  <si>
+    <t>A_Ci=400</t>
+  </si>
+  <si>
+    <t>A_Ca=400</t>
   </si>
 </sst>
 </file>
@@ -8256,9 +8262,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA082BF-324C-409C-9475-FBE41DD98CA6}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N12" sqref="N12:Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8704,10 +8710,10 @@
         <v>6</v>
       </c>
       <c r="N12" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="O12" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="P12" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Updated R and Python code
</commit_message>
<xml_diff>
--- a/Data/A-Ci curves with predicted A-Exp3.xlsx
+++ b/Data/A-Ci curves with predicted A-Exp3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CO2-effects-on-geophytes\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F734322-8382-4E4C-92AD-E3E316FD81CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5804E239-01B9-4590-9985-4B9D2BF022E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{CA5E0E91-9171-4DAE-B053-27BFBA02E87E}"/>
   </bookViews>
@@ -163,19 +163,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2347,19 +2344,19 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H1">
@@ -2388,14 +2385,14 @@
       <c r="C2">
         <v>20</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>-3.263665794342006</v>
       </c>
       <c r="E2">
         <v>8</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
       <c r="H2" t="s">
         <v>0</v>
       </c>
@@ -2429,7 +2426,7 @@
       <c r="W2" t="s">
         <v>0</v>
       </c>
-      <c r="X2" s="4">
+      <c r="X2" s="3">
         <v>0.7</v>
       </c>
       <c r="Y2" t="s">
@@ -2446,7 +2443,7 @@
       <c r="C3">
         <v>20</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>-8.233521777752717E-2</v>
       </c>
       <c r="E3">
@@ -2467,7 +2464,7 @@
       <c r="N3">
         <v>50</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3" s="1">
         <v>-2.0753313758818157</v>
       </c>
       <c r="Q3">
@@ -2504,7 +2501,7 @@
       <c r="C4">
         <v>20</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>5.2361543273481654</v>
       </c>
       <c r="E4">
@@ -2525,7 +2522,7 @@
       <c r="N4">
         <v>100</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="1">
         <v>4.3658285615579331</v>
       </c>
       <c r="Q4">
@@ -2562,7 +2559,7 @@
       <c r="C5">
         <v>20</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>9.5056582073753955</v>
       </c>
       <c r="E5">
@@ -2583,7 +2580,7 @@
       <c r="N5">
         <v>200</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="1">
         <v>15.134040465757517</v>
       </c>
       <c r="Q5">
@@ -2620,7 +2617,7 @@
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>13.0086616809761</v>
       </c>
       <c r="E6">
@@ -2641,7 +2638,7 @@
       <c r="N6">
         <v>300</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="1">
         <v>19.999013847426678</v>
       </c>
       <c r="Q6">
@@ -2678,7 +2675,7 @@
       <c r="C7">
         <v>20</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>15.934576071811794</v>
       </c>
       <c r="E7">
@@ -2699,7 +2696,7 @@
       <c r="N7">
         <v>400</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="1">
         <v>22.374683938440562</v>
       </c>
       <c r="Q7">
@@ -2736,7 +2733,7 @@
       <c r="C8">
         <v>20</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>18.415154350488603</v>
       </c>
       <c r="E8">
@@ -2757,7 +2754,7 @@
       <c r="N8">
         <v>500</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="1">
         <v>23.939247984999849</v>
       </c>
       <c r="Q8">
@@ -2794,7 +2791,7 @@
       <c r="C9">
         <v>20</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>20.54487915616393</v>
       </c>
       <c r="E9">
@@ -2815,7 +2812,7 @@
       <c r="N9">
         <v>600</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="1">
         <v>25.047528122131364</v>
       </c>
       <c r="Q9">
@@ -2852,7 +2849,7 @@
       <c r="C10">
         <v>20</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>22.393271155485856</v>
       </c>
       <c r="E10">
@@ -2873,7 +2870,7 @@
       <c r="N10">
         <v>700</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="1">
         <v>25.873726092219098</v>
       </c>
       <c r="Q10">
@@ -2910,7 +2907,7 @@
       <c r="C11">
         <v>20</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>24.012621874880811</v>
       </c>
       <c r="E11">
@@ -2931,7 +2928,7 @@
       <c r="N11">
         <v>800</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11" s="1">
         <v>26.513378192472313</v>
       </c>
       <c r="Q11">
@@ -2968,7 +2965,7 @@
       <c r="C12">
         <v>20</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>25.443019630196883</v>
       </c>
       <c r="E12">
@@ -2989,7 +2986,7 @@
       <c r="N12">
         <v>900</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="1">
         <v>27.023255161415015</v>
       </c>
       <c r="Q12">
@@ -3026,7 +3023,7 @@
       <c r="C13">
         <v>20</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>-4.0105460906415482</v>
       </c>
       <c r="E13">
@@ -3047,7 +3044,7 @@
       <c r="N13">
         <v>1000</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="1">
         <v>27.439213570766867</v>
       </c>
       <c r="Q13">
@@ -3084,7 +3081,7 @@
       <c r="C14">
         <v>20</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>0.43406724738962232</v>
       </c>
       <c r="E14">
@@ -3101,7 +3098,7 @@
       <c r="C15">
         <v>20</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>7.8644895193096778</v>
       </c>
       <c r="E15">
@@ -3118,7 +3115,7 @@
       <c r="C16">
         <v>20</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>13.829381703647641</v>
       </c>
       <c r="E16">
@@ -3135,7 +3132,7 @@
       <c r="C17">
         <v>20</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>16.146089742463584</v>
       </c>
       <c r="E17">
@@ -3152,7 +3149,7 @@
       <c r="C18">
         <v>20</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>17.427780403957215</v>
       </c>
       <c r="E18">
@@ -3169,7 +3166,7 @@
       <c r="C19">
         <v>20</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>18.335683346763663</v>
       </c>
       <c r="E19">
@@ -3186,7 +3183,7 @@
       <c r="C20">
         <v>20</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>19.012504615368925</v>
       </c>
       <c r="E20">
@@ -3203,7 +3200,7 @@
       <c r="C21">
         <v>20</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>19.536507531901666</v>
       </c>
       <c r="E21">
@@ -3220,7 +3217,7 @@
       <c r="C22">
         <v>20</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>19.95419867790601</v>
       </c>
       <c r="E22">
@@ -3237,7 +3234,7 @@
       <c r="C23">
         <v>20</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>20.294951752226261</v>
       </c>
       <c r="E23">
@@ -3254,7 +3251,7 @@
       <c r="C24">
         <v>20</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="5">
         <v>-2.0753313758818157</v>
       </c>
       <c r="E24">
@@ -3271,7 +3268,7 @@
       <c r="C25">
         <v>20</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="5">
         <v>4.3658285615579331</v>
       </c>
       <c r="E25">
@@ -3288,7 +3285,7 @@
       <c r="C26">
         <v>20</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="5">
         <v>15.134040465757517</v>
       </c>
       <c r="E26">
@@ -3305,7 +3302,7 @@
       <c r="C27">
         <v>20</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="5">
         <v>19.999013847426678</v>
       </c>
       <c r="E27">
@@ -3322,7 +3319,7 @@
       <c r="C28">
         <v>20</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="5">
         <v>22.374683938440562</v>
       </c>
       <c r="E28">
@@ -3339,7 +3336,7 @@
       <c r="C29">
         <v>20</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="5">
         <v>23.939247984999849</v>
       </c>
       <c r="E29">
@@ -3356,7 +3353,7 @@
       <c r="C30">
         <v>20</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="5">
         <v>25.047528122131364</v>
       </c>
       <c r="E30">
@@ -3373,7 +3370,7 @@
       <c r="C31">
         <v>20</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="5">
         <v>25.873726092219098</v>
       </c>
       <c r="E31">
@@ -3390,7 +3387,7 @@
       <c r="C32">
         <v>20</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="5">
         <v>26.513378192472313</v>
       </c>
       <c r="E32">
@@ -3407,7 +3404,7 @@
       <c r="C33">
         <v>20</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="5">
         <v>27.023255161415015</v>
       </c>
       <c r="E33">
@@ -3424,7 +3421,7 @@
       <c r="C34">
         <v>20</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="5">
         <v>27.439213570766867</v>
       </c>
       <c r="E34">
@@ -3441,7 +3438,7 @@
       <c r="C35">
         <v>20</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>-7.3631444039280796</v>
       </c>
       <c r="E35">
@@ -3458,7 +3455,7 @@
       <c r="C36">
         <v>20</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <v>-0.5806060323925637</v>
       </c>
       <c r="E36">
@@ -3475,7 +3472,7 @@
       <c r="C37">
         <v>20</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <v>10.758316016186425</v>
       </c>
       <c r="E37">
@@ -3492,7 +3489,7 @@
       <c r="C38">
         <v>20</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="5">
         <v>16.444946443672485</v>
       </c>
       <c r="E38">
@@ -3509,7 +3506,7 @@
       <c r="C39">
         <v>20</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <v>19.004613416840172</v>
       </c>
       <c r="E39">
@@ -3526,7 +3523,7 @@
       <c r="C40">
         <v>20</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <v>20.69035376123044</v>
       </c>
       <c r="E40">
@@ -3543,7 +3540,7 @@
       <c r="C41">
         <v>20</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="5">
         <v>21.884470770475019</v>
       </c>
       <c r="E41">
@@ -3560,7 +3557,7 @@
       <c r="C42">
         <v>20</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="5">
         <v>22.774658202362588</v>
       </c>
       <c r="E42">
@@ -3577,7 +3574,7 @@
       <c r="C43">
         <v>20</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="5">
         <v>23.463851689930024</v>
       </c>
       <c r="E43">
@@ -3594,7 +3591,7 @@
       <c r="C44">
         <v>20</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="5">
         <v>24.013218894879131</v>
       </c>
       <c r="E44">
@@ -3611,7 +3608,7 @@
       <c r="C45">
         <v>20</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="5">
         <v>24.461393499028354</v>
       </c>
       <c r="E45">
@@ -3628,7 +3625,7 @@
       <c r="C46">
         <v>20</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="5">
         <v>-2.0028964287163236</v>
       </c>
       <c r="E46">
@@ -3645,7 +3642,7 @@
       <c r="C47">
         <v>20</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="5">
         <v>3.6038031759684768</v>
       </c>
       <c r="E47">
@@ -3662,7 +3659,7 @@
       <c r="C48">
         <v>20</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="5">
         <v>12.976979748639589</v>
       </c>
       <c r="E48">
@@ -3679,7 +3676,7 @@
       <c r="C49">
         <v>20</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="5">
         <v>20.501449507516195</v>
       </c>
       <c r="E49">
@@ -3696,7 +3693,7 @@
       <c r="C50">
         <v>20</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="5">
         <v>24.544613416840175</v>
       </c>
       <c r="E50">
@@ -3713,7 +3710,7 @@
       <c r="C51">
         <v>20</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="5">
         <v>26.230353761230443</v>
       </c>
       <c r="E51">
@@ -3730,7 +3727,7 @@
       <c r="C52">
         <v>20</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="5">
         <v>27.424470770475022</v>
       </c>
       <c r="E52">
@@ -3747,7 +3744,7 @@
       <c r="C53">
         <v>20</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53" s="5">
         <v>28.31465820236259</v>
       </c>
       <c r="E53">
@@ -3764,7 +3761,7 @@
       <c r="C54">
         <v>20</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="5">
         <v>29.003851689930027</v>
       </c>
       <c r="E54">
@@ -3781,7 +3778,7 @@
       <c r="C55">
         <v>20</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55" s="5">
         <v>29.55321889487913</v>
       </c>
       <c r="E55">
@@ -3798,7 +3795,7 @@
       <c r="C56">
         <v>20</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56" s="5">
         <v>30.001393499028353</v>
       </c>
       <c r="E56">
@@ -3837,13 +3834,13 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
@@ -3870,7 +3867,7 @@
       <c r="P2" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>0.5</v>
       </c>
     </row>
@@ -3884,7 +3881,7 @@
       <c r="C3">
         <v>20</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>-0.82459462471513212</v>
       </c>
       <c r="E3">
@@ -3923,7 +3920,7 @@
       <c r="C4">
         <v>20</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>2.8739760035096005</v>
       </c>
       <c r="E4">
@@ -3962,7 +3959,7 @@
       <c r="C5">
         <v>20</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>9.0571778886040804</v>
       </c>
       <c r="E5">
@@ -4001,7 +3998,7 @@
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>13.204881848795187</v>
       </c>
       <c r="E6">
@@ -4040,7 +4037,7 @@
       <c r="C7">
         <v>20</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>14.708529165175698</v>
       </c>
       <c r="E7">
@@ -4079,7 +4076,7 @@
       <c r="C8">
         <v>20</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>15.698798200768213</v>
       </c>
       <c r="E8">
@@ -4118,7 +4115,7 @@
       <c r="C9">
         <v>20</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>16.400268687052954</v>
       </c>
       <c r="E9">
@@ -4157,7 +4154,7 @@
       <c r="C10">
         <v>20</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>16.923199192101009</v>
       </c>
       <c r="E10">
@@ -4196,7 +4193,7 @@
       <c r="C11">
         <v>20</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>17.328058085430101</v>
       </c>
       <c r="E11">
@@ -4235,7 +4232,7 @@
       <c r="C12">
         <v>20</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>17.650777615778576</v>
       </c>
       <c r="E12">
@@ -4274,7 +4271,7 @@
       <c r="C13">
         <v>20</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>17.914052701117082</v>
       </c>
       <c r="E13">
@@ -4313,7 +4310,7 @@
       <c r="C14">
         <v>20</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>-4.9890530814402041</v>
       </c>
       <c r="E14">
@@ -4330,19 +4327,19 @@
       <c r="C15">
         <v>20</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>1.166103533316817</v>
       </c>
       <c r="E15">
         <v>17</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I15" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K15" t="s">
@@ -4362,7 +4359,7 @@
       <c r="C16">
         <v>20</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>11.456180378945426</v>
       </c>
       <c r="E16">
@@ -4396,7 +4393,7 @@
       <c r="C17">
         <v>20</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>19.592622861565381</v>
       </c>
       <c r="E17">
@@ -4430,7 +4427,7 @@
       <c r="C18">
         <v>20</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>22.222107894083997</v>
       </c>
       <c r="E18">
@@ -4464,7 +4461,7 @@
       <c r="C19">
         <v>20</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>23.953828876052775</v>
       </c>
       <c r="E19">
@@ -4498,7 +4495,7 @@
       <c r="C20">
         <v>20</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>25.18051689281409</v>
       </c>
       <c r="E20">
@@ -4532,7 +4529,7 @@
       <c r="C21">
         <v>20</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>26.094985279843286</v>
       </c>
       <c r="E21">
@@ -4566,7 +4563,7 @@
       <c r="C22">
         <v>20</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>26.8029773659486</v>
       </c>
       <c r="E22">
@@ -4600,7 +4597,7 @@
       <c r="C23">
         <v>20</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>27.367329235904002</v>
       </c>
       <c r="E23">
@@ -4634,7 +4631,7 @@
       <c r="C24">
         <v>20</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>27.827728352632434</v>
       </c>
       <c r="E24">
@@ -4668,7 +4665,7 @@
       <c r="C25">
         <v>20</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>-0.62124962949276585</v>
       </c>
       <c r="E25">
@@ -4702,7 +4699,7 @@
       <c r="C26">
         <v>20</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>1.6600832571828719</v>
       </c>
       <c r="E26">
@@ -4736,7 +4733,7 @@
       <c r="C27">
         <v>20</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>5.4739733307628677</v>
       </c>
       <c r="E27">
@@ -4753,7 +4750,7 @@
       <c r="C28">
         <v>20</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>8.5356355431236324</v>
       </c>
       <c r="E28">
@@ -4770,7 +4767,7 @@
       <c r="C29">
         <v>20</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>9.6722610988238369</v>
       </c>
       <c r="E29">
@@ -4787,7 +4784,7 @@
       <c r="C30">
         <v>20</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>10.326898645318042</v>
       </c>
       <c r="E30">
@@ -4804,7 +4801,7 @@
       <c r="C31">
         <v>20</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>10.790620019585569</v>
       </c>
       <c r="E31">
@@ -4821,7 +4818,7 @@
       <c r="C32">
         <v>20</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>11.136313897216313</v>
       </c>
       <c r="E32">
@@ -4838,7 +4835,7 @@
       <c r="C33">
         <v>20</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>11.403954127375318</v>
       </c>
       <c r="E33">
@@ -4855,7 +4852,7 @@
       <c r="C34">
         <v>20</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>11.617294456073651</v>
       </c>
       <c r="E34">
@@ -4872,7 +4869,7 @@
       <c r="C35">
         <v>20</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>11.791337821789847</v>
       </c>
       <c r="E35">
@@ -4889,7 +4886,7 @@
       <c r="C36">
         <v>20</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <v>-5.3967249761118321</v>
       </c>
       <c r="E36">
@@ -4906,7 +4903,7 @@
       <c r="C37">
         <v>20</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <v>1.6894637316336443</v>
       </c>
       <c r="E37">
@@ -4923,7 +4920,7 @@
       <c r="C38">
         <v>20</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="5">
         <v>13.536022789206079</v>
       </c>
       <c r="E38">
@@ -4940,7 +4937,7 @@
       <c r="C39">
         <v>20</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <v>19.699559027701923</v>
       </c>
       <c r="E39">
@@ -4957,7 +4954,7 @@
       <c r="C40">
         <v>20</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <v>22.396725341472301</v>
       </c>
       <c r="E40">
@@ -4974,7 +4971,7 @@
       <c r="C41">
         <v>20</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="5">
         <v>24.173019725982158</v>
       </c>
       <c r="E41">
@@ -4991,7 +4988,7 @@
       <c r="C42">
         <v>20</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="5">
         <v>25.431281916258001</v>
       </c>
       <c r="E42">
@@ -5008,7 +5005,7 @@
       <c r="C43">
         <v>20</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="5">
         <v>26.369288141051225</v>
       </c>
       <c r="E43">
@@ -5025,7 +5022,7 @@
       <c r="C44">
         <v>20</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="5">
         <v>27.095503495557434</v>
       </c>
       <c r="E44">
@@ -5042,7 +5039,7 @@
       <c r="C45">
         <v>20</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="5">
         <v>27.674381425620812</v>
       </c>
       <c r="E45">
@@ -5059,7 +5056,7 @@
       <c r="C46">
         <v>20</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="5">
         <v>28.146630924352568</v>
       </c>
       <c r="E46">
@@ -5086,19 +5083,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H1">
@@ -5130,14 +5127,14 @@
       <c r="C2">
         <v>20</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>-11.838711985049889</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
       <c r="H2" t="s">
         <v>0</v>
       </c>
@@ -5171,7 +5168,7 @@
       <c r="W2" t="s">
         <v>0</v>
       </c>
-      <c r="X2" s="4">
+      <c r="X2" s="3">
         <v>1</v>
       </c>
     </row>
@@ -5185,7 +5182,7 @@
       <c r="C3">
         <v>20</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>-3.3918168308132426</v>
       </c>
       <c r="E3">
@@ -5243,7 +5240,7 @@
       <c r="C4">
         <v>20</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>10.729546066058264</v>
       </c>
       <c r="E4">
@@ -5301,7 +5298,7 @@
       <c r="C5">
         <v>20</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>22.065699529915562</v>
       </c>
       <c r="E5">
@@ -5359,7 +5356,7 @@
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>26.907191880741671</v>
       </c>
       <c r="E6">
@@ -5417,7 +5414,7 @@
       <c r="C7">
         <v>20</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>29.370000189797643</v>
       </c>
       <c r="E7">
@@ -5475,7 +5472,7 @@
       <c r="C8">
         <v>20</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>31.114563818555268</v>
       </c>
       <c r="E8">
@@ -5533,7 +5530,7 @@
       <c r="C9">
         <v>20</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>32.415096852106693</v>
       </c>
       <c r="E9">
@@ -5591,7 +5588,7 @@
       <c r="C10">
         <v>20</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>33.421984688289008</v>
       </c>
       <c r="E10">
@@ -5649,7 +5646,7 @@
       <c r="C11">
         <v>20</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>34.224591164175948</v>
       </c>
       <c r="E11">
@@ -5707,7 +5704,7 @@
       <c r="C12">
         <v>20</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>34.879358752007406</v>
       </c>
       <c r="E12">
@@ -5765,7 +5762,7 @@
       <c r="C13">
         <v>20</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>-1.4154233367762785</v>
       </c>
       <c r="E13">
@@ -5823,7 +5820,7 @@
       <c r="C14">
         <v>20</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>5.4176220045095933</v>
       </c>
       <c r="E14">
@@ -5840,7 +5837,7 @@
       <c r="C15">
         <v>20</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>16.840980669814947</v>
       </c>
       <c r="E15">
@@ -5857,7 +5854,7 @@
       <c r="C16">
         <v>20</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>23.599885930450093</v>
       </c>
       <c r="E16">
@@ -5874,7 +5871,7 @@
       <c r="C17">
         <v>20</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>26.2847228445453</v>
       </c>
       <c r="E17">
@@ -5891,7 +5888,7 @@
       <c r="C18">
         <v>20</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>28.052897357731108</v>
       </c>
       <c r="E18">
@@ -5908,7 +5905,7 @@
       <c r="C19">
         <v>20</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>29.305407727156727</v>
       </c>
       <c r="E19">
@@ -5925,7 +5922,7 @@
       <c r="C20">
         <v>20</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>30.239126098589097</v>
       </c>
       <c r="E20">
@@ -5942,7 +5939,7 @@
       <c r="C21">
         <v>20</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>30.962021747035571</v>
       </c>
       <c r="E21">
@@ -5959,7 +5956,7 @@
       <c r="C22">
         <v>20</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>31.538253486047829</v>
       </c>
       <c r="E22">
@@ -5976,7 +5973,7 @@
       <c r="C23">
         <v>20</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>32.008344218081909</v>
       </c>
       <c r="E23">
@@ -5993,7 +5990,7 @@
       <c r="C24">
         <v>20</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>-5.9149606949413496</v>
       </c>
       <c r="E24">
@@ -6010,7 +6007,7 @@
       <c r="C25">
         <v>20</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>5.3080845911326335E-3</v>
       </c>
       <c r="E25">
@@ -6027,7 +6024,7 @@
       <c r="C26">
         <v>20</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>9.9027037970103855</v>
       </c>
       <c r="E26">
@@ -6044,7 +6041,7 @@
       <c r="C27">
         <v>20</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>17.847998986142926</v>
       </c>
       <c r="E27">
@@ -6061,7 +6058,7 @@
       <c r="C28">
         <v>20</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>21.91469362528732</v>
       </c>
       <c r="E28">
@@ -6078,7 +6075,7 @@
       <c r="C29">
         <v>20</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>23.682251210977427</v>
       </c>
       <c r="E29">
@@ -6095,7 +6092,7 @@
       <c r="C30">
         <v>20</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>24.934324571454106</v>
       </c>
       <c r="E30">
@@ -6112,7 +6109,7 @@
       <c r="C31">
         <v>20</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>25.867717162522446</v>
       </c>
       <c r="E31">
@@ -6129,7 +6126,7 @@
       <c r="C32">
         <v>20</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>26.590360588013134</v>
       </c>
       <c r="E32">
@@ -6146,7 +6143,7 @@
       <c r="C33">
         <v>20</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>27.166391276053879</v>
       </c>
       <c r="E33">
@@ -6163,7 +6160,7 @@
       <c r="C34">
         <v>20</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>27.636317990398581</v>
       </c>
       <c r="E34">
@@ -6180,7 +6177,7 @@
       <c r="C35">
         <v>20</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>-1.9769106712523921</v>
       </c>
       <c r="E35">
@@ -6197,7 +6194,7 @@
       <c r="C36">
         <v>20</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <v>5.2388923082620664</v>
       </c>
       <c r="E36">
@@ -6214,7 +6211,7 @@
       <c r="C37">
         <v>20</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <v>17.302138105144323</v>
       </c>
       <c r="E37">
@@ -6231,7 +6228,7 @@
       <c r="C38">
         <v>20</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="5">
         <v>26.986104633331564</v>
       </c>
       <c r="E38">
@@ -6248,7 +6245,7 @@
       <c r="C39">
         <v>20</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <v>30.643153324857202</v>
       </c>
       <c r="E39">
@@ -6265,7 +6262,7 @@
       <c r="C40">
         <v>20</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <v>32.717566097446692</v>
       </c>
       <c r="E40">
@@ -6282,7 +6279,7 @@
       <c r="C41">
         <v>20</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="5">
         <v>34.187004486452736</v>
       </c>
       <c r="E41">
@@ -6299,7 +6296,7 @@
       <c r="C42">
         <v>20</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="5">
         <v>35.282437828160013</v>
       </c>
       <c r="E42">
@@ -6316,7 +6313,7 @@
       <c r="C43">
         <v>20</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="5">
         <v>36.130535091865532</v>
       </c>
       <c r="E43">
@@ -6333,7 +6330,7 @@
       <c r="C44">
         <v>20</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="5">
         <v>36.806567050512406</v>
       </c>
       <c r="E44">
@@ -6350,7 +6347,7 @@
       <c r="C45">
         <v>20</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="5">
         <v>37.358074954022698</v>
       </c>
       <c r="E45">
@@ -6367,7 +6364,7 @@
       <c r="C46">
         <v>20</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="5">
         <v>-1.5893310921455541</v>
       </c>
       <c r="E46">
@@ -6384,7 +6381,7 @@
       <c r="C47">
         <v>20</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="5">
         <v>4.9564938910419167</v>
       </c>
       <c r="E47">
@@ -6401,7 +6398,7 @@
       <c r="C48">
         <v>20</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="5">
         <v>15.899682880505775</v>
       </c>
       <c r="E48">
@@ -6418,7 +6415,7 @@
       <c r="C49">
         <v>20</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="5">
         <v>24.684505611464633</v>
       </c>
       <c r="E49">
@@ -6435,7 +6432,7 @@
       <c r="C50">
         <v>20</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="5">
         <v>29.095939523975886</v>
       </c>
       <c r="E50">
@@ -6452,7 +6449,7 @@
       <c r="C51">
         <v>20</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="5">
         <v>31.045037137323465</v>
       </c>
       <c r="E51">
@@ -6469,7 +6466,7 @@
       <c r="C52">
         <v>20</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="5">
         <v>32.42570683566791</v>
       </c>
       <c r="E52">
@@ -6486,7 +6483,7 @@
       <c r="C53">
         <v>20</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53" s="5">
         <v>33.454965110643613</v>
       </c>
       <c r="E53">
@@ -6503,7 +6500,7 @@
       <c r="C54">
         <v>20</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="5">
         <v>34.251828866216982</v>
       </c>
       <c r="E54">
@@ -6520,7 +6517,7 @@
       <c r="C55">
         <v>20</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55" s="5">
         <v>34.887021772159471</v>
       </c>
       <c r="E55">
@@ -6537,7 +6534,7 @@
       <c r="C56">
         <v>20</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56" s="5">
         <v>35.40521311415182</v>
       </c>
       <c r="E56">
@@ -6561,19 +6558,19 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6587,18 +6584,18 @@
       <c r="C2">
         <v>20</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>-4.5470675560330927</v>
       </c>
-      <c r="E2" s="9">
-        <v>100</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -6610,18 +6607,18 @@
       <c r="C3">
         <v>20</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>2.4452998915182933</v>
       </c>
-      <c r="E3" s="9">
-        <v>100</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -6633,18 +6630,18 @@
       <c r="C4">
         <v>20</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>14.135010303706739</v>
       </c>
-      <c r="E4" s="9">
-        <v>100</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -6656,18 +6653,18 @@
       <c r="C5">
         <v>20</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>23.036838938260956</v>
       </c>
-      <c r="E5" s="9">
-        <v>100</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -6679,18 +6676,18 @@
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>26.969140239881476</v>
       </c>
-      <c r="E6" s="9">
-        <v>100</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -6702,18 +6699,18 @@
       <c r="C7">
         <v>20</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>28.973550398655266</v>
       </c>
-      <c r="E7" s="9">
-        <v>100</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -6725,18 +6722,18 @@
       <c r="C8">
         <v>20</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>30.393401487857354</v>
       </c>
-      <c r="E8" s="9">
-        <v>100</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -6748,18 +6745,18 @@
       <c r="C9">
         <v>20</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>31.451868610404368</v>
       </c>
-      <c r="E9" s="9">
-        <v>100</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -6771,18 +6768,18 @@
       <c r="C10">
         <v>20</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>32.27134619628405</v>
       </c>
-      <c r="E10" s="9">
-        <v>100</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -6794,18 +6791,18 @@
       <c r="C11">
         <v>20</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>32.924564949789904</v>
       </c>
-      <c r="E11" s="9">
-        <v>100</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -6817,18 +6814,18 @@
       <c r="C12">
         <v>20</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>33.457461805732486</v>
       </c>
-      <c r="E12" s="9">
-        <v>100</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -6840,10 +6837,10 @@
       <c r="C13">
         <v>20</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>-3.7431168187019543</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13">
         <v>70</v>
       </c>
     </row>
@@ -6857,10 +6854,10 @@
       <c r="C14">
         <v>20</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>1.5481515469491882</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14">
         <v>70</v>
       </c>
     </row>
@@ -6874,10 +6871,10 @@
       <c r="C15">
         <v>20</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>10.393996015448275</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15">
         <v>70</v>
       </c>
     </row>
@@ -6891,10 +6888,10 @@
       <c r="C16">
         <v>20</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>16.056089941927677</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16">
         <v>70</v>
       </c>
     </row>
@@ -6908,10 +6905,10 @@
       <c r="C17">
         <v>20</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>19.015732439112121</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17">
         <v>70</v>
       </c>
     </row>
@@ -6925,10 +6922,10 @@
       <c r="C18">
         <v>20</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>20.844462396645948</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18">
         <v>70</v>
       </c>
     </row>
@@ -6942,10 +6939,10 @@
       <c r="C19">
         <v>20</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>22.221461472066736</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19">
         <v>70</v>
       </c>
     </row>
@@ -6959,10 +6956,10 @@
       <c r="C20">
         <v>20</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>23.304085253695426</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20">
         <v>70</v>
       </c>
     </row>
@@ -6976,10 +6973,10 @@
       <c r="C21">
         <v>20</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>24.182172051943979</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21">
         <v>70</v>
       </c>
     </row>
@@ -6993,10 +6990,10 @@
       <c r="C22">
         <v>20</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>24.911302700792021</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22">
         <v>70</v>
       </c>
     </row>
@@ -7010,10 +7007,10 @@
       <c r="C23">
         <v>20</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>25.52799439024934</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23">
         <v>70</v>
       </c>
     </row>
@@ -7027,10 +7024,10 @@
       <c r="C24">
         <v>20</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>-2.9579055779399837</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24">
         <v>50</v>
       </c>
     </row>
@@ -7044,10 +7041,10 @@
       <c r="C25">
         <v>20</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>1.8474066314107334</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25">
         <v>50</v>
       </c>
     </row>
@@ -7061,10 +7058,10 @@
       <c r="C26">
         <v>20</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>9.8808385968796131</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26">
         <v>50</v>
       </c>
     </row>
@@ -7078,10 +7075,10 @@
       <c r="C27">
         <v>20</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>15.258174820296531</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27">
         <v>50</v>
       </c>
     </row>
@@ -7095,10 +7092,10 @@
       <c r="C28">
         <v>20</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>17.24990587488896</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28">
         <v>50</v>
       </c>
     </row>
@@ -7112,10 +7109,10 @@
       <c r="C29">
         <v>20</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>18.538136362030297</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29">
         <v>50</v>
       </c>
     </row>
@@ -7129,10 +7126,10 @@
       <c r="C30">
         <v>20</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>19.45067187892765</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30">
         <v>50</v>
       </c>
     </row>
@@ -7146,10 +7143,10 @@
       <c r="C31">
         <v>20</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>20.130946627552959</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31">
         <v>50</v>
       </c>
     </row>
@@ -7163,10 +7160,10 @@
       <c r="C32">
         <v>20</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>20.657623268577865</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32">
         <v>50</v>
       </c>
     </row>
@@ -7180,10 +7177,10 @@
       <c r="C33">
         <v>20</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>21.077445683344258</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33">
         <v>50</v>
       </c>
     </row>
@@ -7197,144 +7194,144 @@
       <c r="C34">
         <v>20</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>21.419937449972984</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34">
         <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D35" s="6"/>
-      <c r="E35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D36" s="6"/>
-      <c r="E36" s="4"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D37" s="6"/>
-      <c r="E37" s="4"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D38" s="6"/>
-      <c r="E38" s="4"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D39" s="6"/>
-      <c r="E39" s="4"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D40" s="6"/>
-      <c r="E40" s="4"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D41" s="6"/>
-      <c r="E41" s="4"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D42" s="6"/>
-      <c r="E42" s="4"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D43" s="6"/>
-      <c r="E43" s="4"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D44" s="6"/>
-      <c r="E44" s="4"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="3"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D45" s="6"/>
-      <c r="E45" s="4"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="3"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D46" s="6"/>
-      <c r="E46" s="4"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D47" s="6"/>
-      <c r="E47" s="4"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="3"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D48" s="6"/>
-      <c r="E48" s="4"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="3"/>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D49" s="6"/>
-      <c r="E49" s="4"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="3"/>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D50" s="6"/>
-      <c r="E50" s="4"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="3"/>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D51" s="6"/>
-      <c r="E51" s="4"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="3"/>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D52" s="6"/>
-      <c r="E52" s="4"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="3"/>
     </row>
     <row r="53" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D53" s="6"/>
-      <c r="E53" s="4"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="3"/>
     </row>
     <row r="54" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D54" s="6"/>
-      <c r="E54" s="4"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="3"/>
     </row>
     <row r="55" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D55" s="6"/>
-      <c r="E55" s="4"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="3"/>
     </row>
     <row r="56" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D56" s="6"/>
-      <c r="E56" s="4"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="3"/>
     </row>
     <row r="57" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D57" s="6"/>
-      <c r="E57" s="4"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="3"/>
     </row>
     <row r="58" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D58" s="6"/>
-      <c r="E58" s="4"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="3"/>
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D59" s="6"/>
-      <c r="E59" s="4"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="3"/>
     </row>
     <row r="60" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D60" s="6"/>
-      <c r="E60" s="4"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="3"/>
     </row>
     <row r="61" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D61" s="6"/>
-      <c r="E61" s="4"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="3"/>
     </row>
     <row r="62" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D62" s="6"/>
-      <c r="E62" s="4"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="3"/>
     </row>
     <row r="63" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D63" s="6"/>
-      <c r="E63" s="4"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="3"/>
     </row>
     <row r="64" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D64" s="6"/>
-      <c r="E64" s="4"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="3"/>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D65" s="6"/>
-      <c r="E65" s="4"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="3"/>
     </row>
     <row r="66" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D66" s="6"/>
-      <c r="E66" s="4"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="3"/>
     </row>
     <row r="67" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D67" s="6"/>
-      <c r="E67" s="4"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7355,10 +7352,10 @@
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
@@ -7399,7 +7396,7 @@
       <c r="D2">
         <v>20</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>-2.9579055779399837</v>
       </c>
       <c r="F2">
@@ -7408,7 +7405,7 @@
       <c r="G2">
         <v>0.89631192968602991</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>0.5</v>
       </c>
       <c r="J2">
@@ -7434,7 +7431,7 @@
       <c r="D3">
         <v>20</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>1.8474066314107334</v>
       </c>
       <c r="F3">
@@ -7443,7 +7440,7 @@
       <c r="G3">
         <v>0.25124128588477962</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>0.7</v>
       </c>
       <c r="J3">
@@ -7469,7 +7466,7 @@
       <c r="D4">
         <v>20</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>9.8808385968796131</v>
       </c>
       <c r="F4">
@@ -7478,7 +7475,7 @@
       <c r="G4">
         <v>1.1990154568848337</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>1</v>
       </c>
       <c r="J4">
@@ -7504,7 +7501,7 @@
       <c r="D5">
         <v>20</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>15.258174820296531</v>
       </c>
       <c r="F5">
@@ -7527,7 +7524,7 @@
       <c r="D6">
         <v>20</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>17.24990587488896</v>
       </c>
       <c r="F6">
@@ -7559,7 +7556,7 @@
       <c r="D7">
         <v>20</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>18.538136362030297</v>
       </c>
       <c r="F7">
@@ -7568,7 +7565,7 @@
       <c r="G7">
         <v>2.3372454040270365</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>0.5</v>
       </c>
       <c r="J7">
@@ -7591,7 +7588,7 @@
       <c r="D8">
         <v>20</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>19.45067187892765</v>
       </c>
       <c r="F8">
@@ -7600,7 +7597,7 @@
       <c r="G8">
         <v>2.4730570405170185</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>0.7</v>
       </c>
       <c r="J8">
@@ -7623,7 +7620,7 @@
       <c r="D9">
         <v>20</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>20.130946627552959</v>
       </c>
       <c r="F9">
@@ -7632,7 +7629,7 @@
       <c r="G9">
         <v>2.574332717022731</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>1</v>
       </c>
       <c r="J9">
@@ -7655,7 +7652,7 @@
       <c r="D10">
         <v>20</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>20.657623268577865</v>
       </c>
       <c r="F10">
@@ -7678,7 +7675,7 @@
       <c r="D11">
         <v>20</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>21.077445683344258</v>
       </c>
       <c r="F11">
@@ -7701,7 +7698,7 @@
       <c r="D12">
         <v>20</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>21.419937449972984</v>
       </c>
       <c r="F12">
@@ -7733,7 +7730,7 @@
       <c r="D13">
         <v>20</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>-3.7431168187019543</v>
       </c>
       <c r="F13">
@@ -7742,7 +7739,7 @@
       <c r="G13">
         <v>0.87671812361904622</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <v>0.5</v>
       </c>
       <c r="J13">
@@ -7765,7 +7762,7 @@
       <c r="D14">
         <v>20</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>1.5481515469491884</v>
       </c>
       <c r="F14">
@@ -7774,7 +7771,7 @@
       <c r="G14">
         <v>0.90766264937196106</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>0.7</v>
       </c>
       <c r="J14">
@@ -7797,7 +7794,7 @@
       <c r="D15">
         <v>20</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>10.393996015448275</v>
       </c>
       <c r="F15">
@@ -7806,7 +7803,7 @@
       <c r="G15">
         <v>1.5782812095857555</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>1</v>
       </c>
       <c r="J15">
@@ -7829,7 +7826,7 @@
       <c r="D16">
         <v>20</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>16.056089941927677</v>
       </c>
       <c r="F16">
@@ -7852,7 +7849,7 @@
       <c r="D17">
         <v>20</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>19.015732439112121</v>
       </c>
       <c r="F17">
@@ -7875,7 +7872,7 @@
       <c r="D18">
         <v>20</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>20.844462396645948</v>
       </c>
       <c r="F18">
@@ -7898,7 +7895,7 @@
       <c r="D19">
         <v>20</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>22.221461472066736</v>
       </c>
       <c r="F19">
@@ -7921,7 +7918,7 @@
       <c r="D20">
         <v>20</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>23.304085253695426</v>
       </c>
       <c r="F20">
@@ -7944,7 +7941,7 @@
       <c r="D21">
         <v>20</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>24.182172051943979</v>
       </c>
       <c r="F21">
@@ -7967,7 +7964,7 @@
       <c r="D22">
         <v>20</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>24.911302700792017</v>
       </c>
       <c r="F22">
@@ -7990,7 +7987,7 @@
       <c r="D23">
         <v>20</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>25.527994390249347</v>
       </c>
       <c r="F23">
@@ -8013,7 +8010,7 @@
       <c r="D24">
         <v>20</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>-4.5470675560330927</v>
       </c>
       <c r="F24">
@@ -8036,7 +8033,7 @@
       <c r="D25">
         <v>20</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>2.4452998915182933</v>
       </c>
       <c r="F25">
@@ -8059,7 +8056,7 @@
       <c r="D26">
         <v>20</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>14.135010303706739</v>
       </c>
       <c r="F26">
@@ -8082,7 +8079,7 @@
       <c r="D27">
         <v>20</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>23.036838938260956</v>
       </c>
       <c r="F27">
@@ -8105,7 +8102,7 @@
       <c r="D28">
         <v>20</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>26.969140239881476</v>
       </c>
       <c r="F28">
@@ -8128,7 +8125,7 @@
       <c r="D29">
         <v>20</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>28.973550398655266</v>
       </c>
       <c r="F29">
@@ -8151,7 +8148,7 @@
       <c r="D30">
         <v>20</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>30.393401487857354</v>
       </c>
       <c r="F30">
@@ -8174,7 +8171,7 @@
       <c r="D31">
         <v>20</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>31.451868610404368</v>
       </c>
       <c r="F31">
@@ -8197,7 +8194,7 @@
       <c r="D32">
         <v>20</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>32.27134619628405</v>
       </c>
       <c r="F32">
@@ -8220,7 +8217,7 @@
       <c r="D33">
         <v>20</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
         <v>32.924564949789904</v>
       </c>
       <c r="F33">
@@ -8243,7 +8240,7 @@
       <c r="D34">
         <v>20</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="5">
         <v>33.457461805732486</v>
       </c>
       <c r="F34">
@@ -8262,13 +8259,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA082BF-324C-409C-9475-FBE41DD98CA6}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N12" sqref="N12:Q25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="10.90625" customWidth="1"/>
     <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
@@ -8278,13 +8276,13 @@
       <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E1" t="s">
@@ -8322,7 +8320,7 @@
       <c r="B2">
         <v>22.34</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <f>'100%'!D6</f>
         <v>26.907191880741671</v>
       </c>
@@ -8367,7 +8365,7 @@
       <c r="B3">
         <v>24.58</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <f>'100%'!D17</f>
         <v>26.2847228445453</v>
       </c>
@@ -8412,7 +8410,7 @@
       <c r="B4">
         <v>18.07</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <f>'100%'!D28</f>
         <v>21.91469362528732</v>
       </c>
@@ -8457,7 +8455,7 @@
       <c r="B5">
         <v>26.97</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <f>'100%'!D39</f>
         <v>30.643153324857202</v>
       </c>
@@ -8491,7 +8489,7 @@
       <c r="B6">
         <v>25.14</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <f>'100%'!D50</f>
         <v>29.095939523975886</v>
       </c>
@@ -8536,7 +8534,7 @@
       <c r="B7">
         <v>14.06</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <f>'70%'!D17</f>
         <v>16.146089742463584</v>
       </c>
@@ -8581,7 +8579,7 @@
       <c r="B8">
         <v>20.86</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <f>'70%'!D28</f>
         <v>22.374683938440562</v>
       </c>
@@ -8617,7 +8615,7 @@
       <c r="B9">
         <v>17.34</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <f>'70%'!D39</f>
         <v>19.004613416840172</v>
       </c>
@@ -8642,7 +8640,7 @@
       <c r="B10">
         <v>20.99</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <f>'70%'!D50</f>
         <v>24.544613416840175</v>
       </c>
@@ -8667,7 +8665,7 @@
       <c r="B11">
         <v>13.38</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <f>'50%'!D7</f>
         <v>14.708529165175698</v>
       </c>
@@ -8692,7 +8690,7 @@
       <c r="B12">
         <v>19.79</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <f>'50%'!D18</f>
         <v>22.222107894083997</v>
       </c>
@@ -8729,7 +8727,7 @@
       <c r="B13">
         <v>8.77</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <f>'50%'!D29</f>
         <v>9.6722610988238369</v>
       </c>
@@ -8766,7 +8764,7 @@
       <c r="B14">
         <v>20.65</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <f>'50%'!D40</f>
         <v>22.396725341472301</v>
       </c>
@@ -8820,7 +8818,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="D16" s="6"/>
+      <c r="D16" s="5"/>
       <c r="J16">
         <v>220.9</v>
       </c>

</xml_diff>